<commit_message>
Updated with new Pst isolates from South Africa
For use with a different project, outside of main marple.
</commit_message>
<xml_diff>
--- a/resources/pst/pst_sample_metadata.xlsx
+++ b/resources/pst/pst_sample_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vof23jop/Documents/MARPLE/marple/resources/pst/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vof23jop/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492F4D5C-38FD-B74A-B6DB-873275944E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37AFBE3-A66E-F84A-B3FB-16A995F786E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17640" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2183" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2576" uniqueCount="864">
   <si>
     <t>tree_name</t>
   </si>
@@ -2273,6 +2273,360 @@
   </si>
   <si>
     <t>[7] UZ189/16: PstS9 v17</t>
+  </si>
+  <si>
+    <t>ERR5960063</t>
+  </si>
+  <si>
+    <t>ERR5960064</t>
+  </si>
+  <si>
+    <t>ERR5960065</t>
+  </si>
+  <si>
+    <t>ERR5960072</t>
+  </si>
+  <si>
+    <t>ERR5960080</t>
+  </si>
+  <si>
+    <t>ERR5960081</t>
+  </si>
+  <si>
+    <t>ERR5960082</t>
+  </si>
+  <si>
+    <t>ERR5960086</t>
+  </si>
+  <si>
+    <t>ERR5960059</t>
+  </si>
+  <si>
+    <t>ERR5960060</t>
+  </si>
+  <si>
+    <t>ERR5960061</t>
+  </si>
+  <si>
+    <t>ERR5960062</t>
+  </si>
+  <si>
+    <t>ERR5960067</t>
+  </si>
+  <si>
+    <t>ERR5960068</t>
+  </si>
+  <si>
+    <t>ERR5960069</t>
+  </si>
+  <si>
+    <t>ERR5960075</t>
+  </si>
+  <si>
+    <t>ERR5960076</t>
+  </si>
+  <si>
+    <t>ERR5960077</t>
+  </si>
+  <si>
+    <t>ERR5960083</t>
+  </si>
+  <si>
+    <t>ERR5960066</t>
+  </si>
+  <si>
+    <t>ERR5960070</t>
+  </si>
+  <si>
+    <t>ERR5960071</t>
+  </si>
+  <si>
+    <t>ERR5960073</t>
+  </si>
+  <si>
+    <t>ERR5960074</t>
+  </si>
+  <si>
+    <t>ERR5960078</t>
+  </si>
+  <si>
+    <t>ERR5960079</t>
+  </si>
+  <si>
+    <t>ERR5960084</t>
+  </si>
+  <si>
+    <t>ERR5960085</t>
+  </si>
+  <si>
+    <t>ERR3856852</t>
+  </si>
+  <si>
+    <t>ERR3856851</t>
+  </si>
+  <si>
+    <t>ERR3856850</t>
+  </si>
+  <si>
+    <t>ERR3856849</t>
+  </si>
+  <si>
+    <t>ERR3856848</t>
+  </si>
+  <si>
+    <t>ERR3856847</t>
+  </si>
+  <si>
+    <t>ERR3856846</t>
+  </si>
+  <si>
+    <t>ERR3856845</t>
+  </si>
+  <si>
+    <t>ERR3856855</t>
+  </si>
+  <si>
+    <t>ERR3856854</t>
+  </si>
+  <si>
+    <t>ERR3856853</t>
+  </si>
+  <si>
+    <t>ERR3856844</t>
+  </si>
+  <si>
+    <t>ERR3856843</t>
+  </si>
+  <si>
+    <t>ERR3856842</t>
+  </si>
+  <si>
+    <t>ERR3856840</t>
+  </si>
+  <si>
+    <t>ERR3856839</t>
+  </si>
+  <si>
+    <t>ERR3856838</t>
+  </si>
+  <si>
+    <t>ERR3856837</t>
+  </si>
+  <si>
+    <t>ERR3856836</t>
+  </si>
+  <si>
+    <t>ERR3856835</t>
+  </si>
+  <si>
+    <t>ERR3856834</t>
+  </si>
+  <si>
+    <t>ERR3856833</t>
+  </si>
+  <si>
+    <t>ERR3856832</t>
+  </si>
+  <si>
+    <t>ERR3856831</t>
+  </si>
+  <si>
+    <t>ERR3856830</t>
+  </si>
+  <si>
+    <t>ERR3856841</t>
+  </si>
+  <si>
+    <t>20.0308</t>
+  </si>
+  <si>
+    <t>20.0309</t>
+  </si>
+  <si>
+    <t>20.0310</t>
+  </si>
+  <si>
+    <t>20.0331</t>
+  </si>
+  <si>
+    <t>20.0326</t>
+  </si>
+  <si>
+    <t>20.0299</t>
+  </si>
+  <si>
+    <t>20.0315</t>
+  </si>
+  <si>
+    <t>20.0329</t>
+  </si>
+  <si>
+    <t>20.0297</t>
+  </si>
+  <si>
+    <t>20.0302</t>
+  </si>
+  <si>
+    <t>20.0304</t>
+  </si>
+  <si>
+    <t>20.0307</t>
+  </si>
+  <si>
+    <t>20.0312</t>
+  </si>
+  <si>
+    <t>20.0313</t>
+  </si>
+  <si>
+    <t>20.0318</t>
+  </si>
+  <si>
+    <t>20.0334</t>
+  </si>
+  <si>
+    <t>20.0335</t>
+  </si>
+  <si>
+    <t>20.0322</t>
+  </si>
+  <si>
+    <t>20.0300</t>
+  </si>
+  <si>
+    <t>20.0311</t>
+  </si>
+  <si>
+    <t>20.0321</t>
+  </si>
+  <si>
+    <t>20.0330</t>
+  </si>
+  <si>
+    <t>20.0332</t>
+  </si>
+  <si>
+    <t>20.0333</t>
+  </si>
+  <si>
+    <t>20.0323</t>
+  </si>
+  <si>
+    <t>20.0324</t>
+  </si>
+  <si>
+    <t>20.0316</t>
+  </si>
+  <si>
+    <t>20.0327</t>
+  </si>
+  <si>
+    <t>15/SAZP9</t>
+  </si>
+  <si>
+    <t>15/SAZP8</t>
+  </si>
+  <si>
+    <t>15/SAZP7</t>
+  </si>
+  <si>
+    <t>15/SAZP6</t>
+  </si>
+  <si>
+    <t>15/SAZP5</t>
+  </si>
+  <si>
+    <t>15/SAZP4</t>
+  </si>
+  <si>
+    <t>15/SAZP3</t>
+  </si>
+  <si>
+    <t>15/SAZP2</t>
+  </si>
+  <si>
+    <t>15/SAZP12</t>
+  </si>
+  <si>
+    <t>15/SAZP11</t>
+  </si>
+  <si>
+    <t>15/SAZP10</t>
+  </si>
+  <si>
+    <t>15/SAZP1</t>
+  </si>
+  <si>
+    <t>14/SAZP3</t>
+  </si>
+  <si>
+    <t>14/SAZP2</t>
+  </si>
+  <si>
+    <t>14/SATT5</t>
+  </si>
+  <si>
+    <t>14/SATT4</t>
+  </si>
+  <si>
+    <t>14/SATT3</t>
+  </si>
+  <si>
+    <t>14/SATT2</t>
+  </si>
+  <si>
+    <t>14/SATT1</t>
+  </si>
+  <si>
+    <t>14/SADL6</t>
+  </si>
+  <si>
+    <t>14/SADL5</t>
+  </si>
+  <si>
+    <t>14/SADL4</t>
+  </si>
+  <si>
+    <t>14/SADL3</t>
+  </si>
+  <si>
+    <t>14/SADL2</t>
+  </si>
+  <si>
+    <t>14/SADL1</t>
+  </si>
+  <si>
+    <t>13/SAZP1</t>
+  </si>
+  <si>
+    <t>Schalkwyk et al. 2021</t>
+  </si>
+  <si>
+    <t>SA Collection</t>
+  </si>
+  <si>
+    <t>SA Collection (6E22A+)</t>
+  </si>
+  <si>
+    <t>SA Collection (6E16A-)</t>
+  </si>
+  <si>
+    <t>SA Collection (6E22A-)</t>
+  </si>
+  <si>
+    <t>#AF8050</t>
+  </si>
+  <si>
+    <t>#D69C29</t>
+  </si>
+  <si>
+    <t>#2963D6</t>
+  </si>
+  <si>
+    <t>#C4D22D</t>
+  </si>
+  <si>
+    <t>★</t>
   </si>
 </sst>
 </file>
@@ -2301,7 +2655,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="61">
+  <fills count="65">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2662,6 +3016,30 @@
         <bgColor rgb="FF76C500"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB08050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD69C28"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3162D6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC4D22D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -2690,7 +3068,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2753,6 +3131,10 @@
     <xf numFmtId="0" fontId="0" fillId="59" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="60" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="61" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="62" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2826,6 +3208,12 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFC4D22D"/>
+      <color rgb="FF3162D6"/>
+      <color rgb="FFD69C28"/>
+      <color rgb="FFB08050"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3014,11 +3402,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H270"/>
+  <dimension ref="A1:H324"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A311" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D324" sqref="D324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9493,6 +9881,1248 @@
         <v>731</v>
       </c>
     </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A271" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D271" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E271" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F271" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H271" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A272" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F272" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H272" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A273" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D273" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F273" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H273" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A274" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D274" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F274" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H274" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A275" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D275" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E275" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F275" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H275" s="1" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A276" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D276" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E276" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F276" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H276" s="1" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A277" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E277" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F277" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H277" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A278" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D278" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E278" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F278" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H278" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A279" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D279" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F279" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H279" s="1" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A280" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E280" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F280" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H280" s="1" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A281" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E281" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F281" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H281" s="1" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A282" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E282" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F282" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H282" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A283" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E283" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F283" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H283" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A284" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D284" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E284" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F284" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H284" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A285" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D285" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E285" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F285" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H285" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="286" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A286" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D286" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E286" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F286" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H286" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A287" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D287" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E287" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F287" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H287" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="288" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A288" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D288" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E288" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F288" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H288" s="1" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A289" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D289" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E289" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F289" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H289" s="1" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="290" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A290" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D290" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E290" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F290" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H290" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A291" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E291" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F291" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H291" s="1" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="292" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A292" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D292" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E292" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F292" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H292" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="293" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A293" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D293" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E293" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F293" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H293" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="294" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A294" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D294" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E294" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F294" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H294" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="295" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A295" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D295" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E295" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F295" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H295" s="1" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="296" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A296" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D296" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E296" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F296" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H296" s="1" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="297" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A297" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D297" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E297" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F297" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H297" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="298" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A298" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D298" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E298" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F298" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H298" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="299" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A299" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D299" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E299" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F299" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H299" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="300" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A300" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B300" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D300" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E300" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F300" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H300" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="301" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A301" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D301" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E301" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F301" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H301" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A302" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D302" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E302" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F302" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H302" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="303" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A303" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D303" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E303" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F303" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H303" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="304" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A304" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D304" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E304" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F304" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H304" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="305" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A305" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="B305" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D305" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E305" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F305" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H305" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="306" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A306" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B306" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D306" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E306" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F306" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H306" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="307" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A307" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D307" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E307" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F307" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H307" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="308" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A308" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D308" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E308" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F308" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H308" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="309" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A309" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D309" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E309" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F309" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H309" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="310" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A310" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D310" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E310" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F310" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H310" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="311" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A311" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="C311" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D311" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E311" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F311" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H311" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="312" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A312" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D312" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E312" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F312" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H312" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="313" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A313" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="C313" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D313" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E313" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F313" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H313" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="314" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A314" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="C314" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D314" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E314" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F314" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H314" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="315" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A315" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D315" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E315" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F315" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H315" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="316" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A316" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D316" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E316" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F316" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H316" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="317" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A317" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D317" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E317" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F317" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H317" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="318" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A318" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D318" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E318" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F318" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H318" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="319" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A319" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D319" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E319" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F319" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H319" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="320" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A320" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D320" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E320" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F320" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H320" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="321" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A321" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D321" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E321" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F321" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H321" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="322" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A322" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D322" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E322" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F322" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H322" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="323" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A323" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D323" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E323" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F323" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H323" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="324" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A324" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="C324" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D324" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E324" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F324" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="H324" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H269" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H269">
@@ -9506,9 +11136,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="132" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:C22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9713,6 +11345,50 @@
       </c>
       <c r="C18" s="2" t="s">
         <v>680</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="B19" s="62" t="s">
+        <v>859</v>
+      </c>
+      <c r="C19" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="B20" s="63" t="s">
+        <v>860</v>
+      </c>
+      <c r="C20" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="B21" s="64" t="s">
+        <v>861</v>
+      </c>
+      <c r="C21" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="B22" s="65" t="s">
+        <v>862</v>
+      </c>
+      <c r="C22" t="s">
+        <v>863</v>
       </c>
     </row>
   </sheetData>
@@ -10078,9 +11754,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10320,6 +11998,17 @@
         <v>663</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="B22" s="65" t="s">
+        <v>862</v>
+      </c>
+      <c r="C22" t="s">
+        <v>863</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>